<commit_message>
++ modified advertising xlsx file
</commit_message>
<xml_diff>
--- a/Datasets/Advertising.xlsx
+++ b/Datasets/Advertising.xlsx
@@ -1,108 +1,431 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\Working_Enviroment\Data_Analytics\Datasets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBE7696-F181-4823-B4AE-4E40EF45BDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Advertising" sheetId="1" r:id="rId3"/>
+    <sheet name="Advertising" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>TV</t>
+    <t>id</t>
   </si>
   <si>
-    <t>Radio</t>
+    <t>tv</t>
   </si>
   <si>
-    <t>Newspaper</t>
+    <t>radio</t>
   </si>
   <si>
-    <t>Sales</t>
+    <t>newspaper</t>
+  </si>
+  <si>
+    <t>sales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
       </c>
       <c r="B2" s="1">
         <v>230.1</v>
       </c>
       <c r="C2" s="1">
-        <v>37.8</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="D2" s="1">
         <v>69.2</v>
@@ -111,15 +434,15 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>44.5</v>
       </c>
       <c r="C3" s="1">
-        <v>39.3</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="D3" s="1">
         <v>45.1</v>
@@ -128,9 +451,9 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>17.2</v>
@@ -142,12 +465,12 @@
         <v>69.3</v>
       </c>
       <c r="E4" s="1">
-        <v>9.3</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>151.5</v>
@@ -162,9 +485,9 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>180.8</v>
@@ -179,32 +502,32 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C7" s="1">
         <v>48.9</v>
       </c>
       <c r="D7" s="1">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1">
         <v>7.2</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>57.5</v>
       </c>
       <c r="C8" s="1">
-        <v>32.8</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="D8" s="1">
         <v>23.5</v>
@@ -213,15 +536,15 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>120.2</v>
       </c>
       <c r="C9" s="1">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="D9" s="1">
         <v>11.6</v>
@@ -230,9 +553,9 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>8.6</v>
@@ -241,15 +564,15 @@
         <v>2.1</v>
       </c>
       <c r="D10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
         <v>4.8</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>199.8</v>
@@ -264,12 +587,12 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>66.1</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="C12" s="1">
         <v>5.8</v>
@@ -281,26 +604,26 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>214.7</v>
       </c>
       <c r="C13" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E13" s="1">
-        <v>17.4</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>23.8</v>
@@ -309,15 +632,15 @@
         <v>35.1</v>
       </c>
       <c r="D14" s="1">
-        <v>65.9</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="E14" s="1">
-        <v>9.2</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>97.5</v>
@@ -329,12 +652,12 @@
         <v>7.2</v>
       </c>
       <c r="E15" s="1">
-        <v>9.7</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>204.1</v>
@@ -343,15 +666,15 @@
         <v>32.9</v>
       </c>
       <c r="D16" s="1">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="E16" s="1">
-        <v>19.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>195.4</v>
@@ -366,9 +689,9 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>67.8</v>
@@ -377,18 +700,18 @@
         <v>36.6</v>
       </c>
       <c r="D18" s="1">
-        <v>114.0</v>
+        <v>114</v>
       </c>
       <c r="E18" s="1">
         <v>12.5</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>281.4</v>
+        <v>281.39999999999998</v>
       </c>
       <c r="C19" s="1">
         <v>39.6</v>
@@ -400,9 +723,9 @@
         <v>24.4</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>69.2</v>
@@ -417,26 +740,26 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>147.3</v>
+        <v>147.30000000000001</v>
       </c>
       <c r="C21" s="1">
         <v>23.9</v>
       </c>
       <c r="D21" s="1">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E21" s="1">
         <v>14.6</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>218.4</v>
@@ -448,18 +771,18 @@
         <v>53.4</v>
       </c>
       <c r="E22" s="1">
-        <v>18.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>237.4</v>
       </c>
       <c r="C23" s="1">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D23" s="1">
         <v>23.5</v>
@@ -468,9 +791,9 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>13.2</v>
@@ -485,15 +808,15 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>228.3</v>
       </c>
       <c r="C25" s="1">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="D25" s="1">
         <v>26.2</v>
@@ -502,9 +825,9 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>62.3</v>
@@ -516,15 +839,15 @@
         <v>18.3</v>
       </c>
       <c r="E26" s="1">
-        <v>9.7</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>262.9</v>
+        <v>262.89999999999998</v>
       </c>
       <c r="C27" s="1">
         <v>3.5</v>
@@ -533,12 +856,12 @@
         <v>19.5</v>
       </c>
       <c r="E27" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>142.9</v>
@@ -550,12 +873,12 @@
         <v>12.6</v>
       </c>
       <c r="E28" s="1">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>240.1</v>
@@ -570,9 +893,9 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>248.8</v>
@@ -584,32 +907,32 @@
         <v>22.9</v>
       </c>
       <c r="E30" s="1">
-        <v>18.9</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>70.6</v>
+        <v>70.599999999999994</v>
       </c>
       <c r="C31" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="D31" s="1">
-        <v>40.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="E31" s="1">
         <v>10.5</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>292.9</v>
+        <v>292.89999999999998</v>
       </c>
       <c r="C32" s="1">
         <v>28.3</v>
@@ -621,15 +944,15 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1">
         <v>112.9</v>
       </c>
       <c r="C33" s="1">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="D33" s="1">
         <v>38.6</v>
@@ -638,9 +961,9 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1">
         <v>97.2</v>
@@ -649,32 +972,32 @@
         <v>1.5</v>
       </c>
       <c r="D34" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="E34" s="1">
         <v>9.6</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>265.6</v>
+        <v>265.60000000000002</v>
       </c>
       <c r="C35" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D35" s="1">
         <v>0.3</v>
       </c>
       <c r="E35" s="1">
-        <v>17.4</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>95.7</v>
@@ -689,15 +1012,15 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>290.7</v>
       </c>
       <c r="C37" s="1">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D37" s="1">
         <v>8.5</v>
@@ -706,26 +1029,26 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>266.9</v>
+        <v>266.89999999999998</v>
       </c>
       <c r="C38" s="1">
         <v>43.8</v>
       </c>
       <c r="D38" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E38" s="1">
         <v>25.4</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1">
         <v>74.7</v>
@@ -740,9 +1063,9 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1">
         <v>43.1</v>
@@ -757,26 +1080,26 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>228.0</v>
+        <v>228</v>
       </c>
       <c r="C41" s="1">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="D41" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="E41" s="1">
         <v>21.5</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>202.5</v>
@@ -788,32 +1111,32 @@
         <v>31.6</v>
       </c>
       <c r="E42" s="1">
-        <v>16.6</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1">
-        <v>177.0</v>
+        <v>177</v>
       </c>
       <c r="C43" s="1">
         <v>33.4</v>
       </c>
       <c r="D43" s="1">
-        <v>38.7</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="E43" s="1">
-        <v>17.1</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1">
-        <v>293.6</v>
+        <v>293.60000000000002</v>
       </c>
       <c r="C44" s="1">
         <v>27.7</v>
@@ -825,9 +1148,9 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1">
         <v>206.9</v>
@@ -842,9 +1165,9 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1">
         <v>25.1</v>
@@ -859,9 +1182,9 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1">
         <v>175.1</v>
@@ -876,9 +1199,9 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1">
         <v>89.7</v>
@@ -887,15 +1210,15 @@
         <v>9.9</v>
       </c>
       <c r="D48" s="1">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="E48" s="1">
         <v>10.6</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1">
         <v>239.9</v>
@@ -910,9 +1233,9 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1">
         <v>227.2</v>
@@ -927,26 +1250,26 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1">
-        <v>66.9</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="C51" s="1">
         <v>11.7</v>
       </c>
       <c r="D51" s="1">
-        <v>36.8</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="E51" s="1">
-        <v>9.7</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1">
         <v>199.8</v>
@@ -961,9 +1284,9 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1">
         <v>100.4</v>
@@ -978,9 +1301,9 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1">
         <v>216.4</v>
@@ -995,9 +1318,9 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1">
         <v>182.6</v>
@@ -1012,9 +1335,9 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1">
         <v>262.7</v>
@@ -1029,9 +1352,9 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1">
         <v>198.9</v>
@@ -1040,15 +1363,15 @@
         <v>49.4</v>
       </c>
       <c r="D57" s="1">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="E57" s="1">
         <v>23.7</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1">
         <v>7.3</v>
@@ -1063,26 +1386,26 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1">
-        <v>136.2</v>
+        <v>136.19999999999999</v>
       </c>
       <c r="C59" s="1">
         <v>19.2</v>
       </c>
       <c r="D59" s="1">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="E59" s="1">
         <v>13.2</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1">
         <v>210.8</v>
@@ -1091,15 +1414,15 @@
         <v>49.6</v>
       </c>
       <c r="D60" s="1">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="E60" s="1">
         <v>23.8</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="B61" s="1">
         <v>210.7</v>
@@ -1108,21 +1431,21 @@
         <v>29.5</v>
       </c>
       <c r="D61" s="1">
-        <v>9.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E61" s="1">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="B62" s="1">
         <v>53.5</v>
       </c>
       <c r="C62" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D62" s="1">
         <v>21.4</v>
@@ -1131,9 +1454,9 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="B63" s="1">
         <v>261.3</v>
@@ -1148,9 +1471,9 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1">
         <v>239.3</v>
@@ -1165,9 +1488,9 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="B65" s="1">
         <v>102.7</v>
@@ -1179,12 +1502,12 @@
         <v>8.4</v>
       </c>
       <c r="E65" s="1">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="B66" s="1">
         <v>131.1</v>
@@ -1196,29 +1519,29 @@
         <v>28.9</v>
       </c>
       <c r="E66" s="1">
-        <v>18.0</v>
-      </c>
-    </row>
-    <row r="67">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>66.0</v>
+        <v>66</v>
       </c>
       <c r="B67" s="1">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="C67" s="1">
-        <v>9.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D67" s="1">
         <v>0.9</v>
       </c>
       <c r="E67" s="1">
-        <v>9.3</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>67.0</v>
+        <v>67</v>
       </c>
       <c r="B68" s="1">
         <v>31.5</v>
@@ -1227,32 +1550,32 @@
         <v>24.6</v>
       </c>
       <c r="D68" s="1">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E68" s="1">
         <v>9.5</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="B69" s="1">
-        <v>139.3</v>
+        <v>139.30000000000001</v>
       </c>
       <c r="C69" s="1">
         <v>14.5</v>
       </c>
       <c r="D69" s="1">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="E69" s="1">
         <v>13.4</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="B70" s="1">
         <v>237.4</v>
@@ -1261,15 +1584,15 @@
         <v>27.5</v>
       </c>
       <c r="D70" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="E70" s="1">
-        <v>18.9</v>
-      </c>
-    </row>
-    <row r="71">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="B71" s="1">
         <v>216.8</v>
@@ -1284,9 +1607,9 @@
         <v>22.3</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1">
         <v>199.1</v>
@@ -1295,15 +1618,15 @@
         <v>30.6</v>
       </c>
       <c r="D72" s="1">
-        <v>38.7</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="E72" s="1">
         <v>18.3</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1">
         <v>109.8</v>
@@ -1318,26 +1641,26 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="B74" s="1">
         <v>26.8</v>
       </c>
       <c r="C74" s="1">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="D74" s="1">
         <v>19.3</v>
       </c>
       <c r="E74" s="1">
-        <v>8.8</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="B75" s="1">
         <v>129.4</v>
@@ -1349,12 +1672,12 @@
         <v>31.3</v>
       </c>
       <c r="E75" s="1">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="76">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="B76" s="1">
         <v>213.4</v>
@@ -1366,15 +1689,15 @@
         <v>13.1</v>
       </c>
       <c r="E76" s="1">
-        <v>17.0</v>
-      </c>
-    </row>
-    <row r="77">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>76.0</v>
+        <v>76</v>
       </c>
       <c r="B77" s="1">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="C77" s="1">
         <v>43.7</v>
@@ -1383,12 +1706,12 @@
         <v>89.4</v>
       </c>
       <c r="E77" s="1">
-        <v>8.7</v>
-      </c>
-    </row>
-    <row r="78">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="B78" s="1">
         <v>27.5</v>
@@ -1403,9 +1726,9 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="B79" s="1">
         <v>120.5</v>
@@ -1420,9 +1743,9 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="B80" s="1">
         <v>5.4</v>
@@ -1437,12 +1760,12 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="B81" s="1">
-        <v>116.0</v>
+        <v>116</v>
       </c>
       <c r="C81" s="1">
         <v>7.7</v>
@@ -1451,15 +1774,15 @@
         <v>23.1</v>
       </c>
       <c r="E81" s="1">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="82">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>81.0</v>
+        <v>81</v>
       </c>
       <c r="B82" s="1">
-        <v>76.4</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="C82" s="1">
         <v>26.7</v>
@@ -1471,15 +1794,15 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="B83" s="1">
         <v>239.8</v>
       </c>
       <c r="C83" s="1">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D83" s="1">
         <v>36.9</v>
@@ -1488,9 +1811,9 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="B84" s="1">
         <v>75.3</v>
@@ -1505,12 +1828,12 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="B85" s="1">
-        <v>68.4</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="C85" s="1">
         <v>44.5</v>
@@ -1522,32 +1845,32 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="B86" s="1">
         <v>213.5</v>
       </c>
       <c r="C86" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="D86" s="1">
-        <v>33.8</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="E86" s="1">
         <v>21.7</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>86.0</v>
+        <v>86</v>
       </c>
       <c r="B87" s="1">
         <v>193.2</v>
       </c>
       <c r="C87" s="1">
-        <v>18.4</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="D87" s="1">
         <v>65.7</v>
@@ -1556,9 +1879,9 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>87.0</v>
+        <v>87</v>
       </c>
       <c r="B88" s="1">
         <v>76.3</v>
@@ -1567,15 +1890,15 @@
         <v>27.5</v>
       </c>
       <c r="D88" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="E88" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="89">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>88.0</v>
+        <v>88</v>
       </c>
       <c r="B89" s="1">
         <v>110.7</v>
@@ -1587,12 +1910,12 @@
         <v>63.2</v>
       </c>
       <c r="E89" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>89.0</v>
+        <v>89</v>
       </c>
       <c r="B90" s="1">
         <v>88.3</v>
@@ -1601,15 +1924,15 @@
         <v>25.5</v>
       </c>
       <c r="D90" s="1">
-        <v>73.4</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="E90" s="1">
         <v>12.9</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="B91" s="1">
         <v>109.8</v>
@@ -1624,26 +1947,26 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>91.0</v>
+        <v>91</v>
       </c>
       <c r="B92" s="1">
-        <v>134.3</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="C92" s="1">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D92" s="1">
-        <v>9.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E92" s="1">
         <v>11.2</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>92.0</v>
+        <v>92</v>
       </c>
       <c r="B93" s="1">
         <v>28.6</v>
@@ -1652,15 +1975,15 @@
         <v>1.5</v>
       </c>
       <c r="D93" s="1">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="E93" s="1">
         <v>7.3</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>93.0</v>
+        <v>93</v>
       </c>
       <c r="B94" s="1">
         <v>217.7</v>
@@ -1669,15 +1992,15 @@
         <v>33.5</v>
       </c>
       <c r="D94" s="1">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="E94" s="1">
-        <v>19.4</v>
-      </c>
-    </row>
-    <row r="95">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="B95" s="1">
         <v>250.9</v>
@@ -1692,15 +2015,15 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>95.0</v>
+        <v>95</v>
       </c>
       <c r="B96" s="1">
         <v>107.4</v>
       </c>
       <c r="C96" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="D96" s="1">
         <v>10.9</v>
@@ -1709,12 +2032,12 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="B97" s="1">
-        <v>163.3</v>
+        <v>163.30000000000001</v>
       </c>
       <c r="C97" s="1">
         <v>31.6</v>
@@ -1723,12 +2046,12 @@
         <v>52.9</v>
       </c>
       <c r="E97" s="1">
-        <v>16.9</v>
-      </c>
-    </row>
-    <row r="98">
+        <v>16.899999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="B98" s="1">
         <v>197.6</v>
@@ -1743,26 +2066,26 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="B99" s="1">
         <v>184.9</v>
       </c>
       <c r="C99" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D99" s="1">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="E99" s="1">
         <v>15.5</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="B100" s="1">
         <v>289.7</v>
@@ -1777,12 +2100,12 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="B101" s="1">
-        <v>135.2</v>
+        <v>135.19999999999999</v>
       </c>
       <c r="C101" s="1">
         <v>41.7</v>
@@ -1794,9 +2117,9 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="B102" s="1">
         <v>222.4</v>
@@ -1811,15 +2134,15 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="B103" s="1">
-        <v>296.4</v>
+        <v>296.39999999999998</v>
       </c>
       <c r="C103" s="1">
-        <v>36.3</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="D103" s="1">
         <v>100.9</v>
@@ -1828,9 +2151,9 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="B104" s="1">
         <v>280.2</v>
@@ -1845,9 +2168,9 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="B105" s="1">
         <v>187.9</v>
@@ -1856,21 +2179,21 @@
         <v>17.2</v>
       </c>
       <c r="D105" s="1">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="E105" s="1">
         <v>14.7</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="B106" s="1">
         <v>238.2</v>
       </c>
       <c r="C106" s="1">
-        <v>34.3</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="D106" s="1">
         <v>5.3</v>
@@ -1879,9 +2202,9 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>106.0</v>
+        <v>106</v>
       </c>
       <c r="B107" s="1">
         <v>137.9</v>
@@ -1890,21 +2213,21 @@
         <v>46.4</v>
       </c>
       <c r="D107" s="1">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="E107" s="1">
         <v>19.2</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>107.0</v>
+        <v>107</v>
       </c>
       <c r="B108" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="C108" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="D108" s="1">
         <v>29.7</v>
@@ -1913,9 +2236,9 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>108.0</v>
+        <v>108</v>
       </c>
       <c r="B109" s="1">
         <v>90.4</v>
@@ -1927,12 +2250,12 @@
         <v>23.2</v>
       </c>
       <c r="E109" s="1">
-        <v>8.7</v>
-      </c>
-    </row>
-    <row r="110">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>109.0</v>
+        <v>109</v>
       </c>
       <c r="B110" s="1">
         <v>13.1</v>
@@ -1947,9 +2270,9 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="B111" s="1">
         <v>255.4</v>
@@ -1964,15 +2287,15 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>111.0</v>
+        <v>111</v>
       </c>
       <c r="B112" s="1">
         <v>225.8</v>
       </c>
       <c r="C112" s="1">
-        <v>8.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D112" s="1">
         <v>56.5</v>
@@ -1981,15 +2304,15 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>112.0</v>
+        <v>112</v>
       </c>
       <c r="B113" s="1">
         <v>241.7</v>
       </c>
       <c r="C113" s="1">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="D113" s="1">
         <v>23.2</v>
@@ -1998,9 +2321,9 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>113.0</v>
+        <v>113</v>
       </c>
       <c r="B114" s="1">
         <v>175.7</v>
@@ -2015,9 +2338,9 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>114.0</v>
+        <v>114</v>
       </c>
       <c r="B115" s="1">
         <v>209.6</v>
@@ -2032,9 +2355,9 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>115.0</v>
+        <v>115</v>
       </c>
       <c r="B116" s="1">
         <v>78.2</v>
@@ -2049,15 +2372,15 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>116.0</v>
+        <v>116</v>
       </c>
       <c r="B117" s="1">
-        <v>75.1</v>
+        <v>75.099999999999994</v>
       </c>
       <c r="C117" s="1">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="D117" s="1">
         <v>52.7</v>
@@ -2066,12 +2389,12 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>117.0</v>
+        <v>117</v>
       </c>
       <c r="B118" s="1">
-        <v>139.2</v>
+        <v>139.19999999999999</v>
       </c>
       <c r="C118" s="1">
         <v>14.3</v>
@@ -2083,12 +2406,12 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>118.0</v>
+        <v>118</v>
       </c>
       <c r="B119" s="1">
-        <v>76.4</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="C119" s="1">
         <v>0.8</v>
@@ -2100,9 +2423,9 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>119.0</v>
+        <v>119</v>
       </c>
       <c r="B120" s="1">
         <v>125.7</v>
@@ -2117,15 +2440,15 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="B121" s="1">
-        <v>19.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="C121" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="D121" s="1">
         <v>22.3</v>
@@ -2134,12 +2457,12 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>121.0</v>
+        <v>121</v>
       </c>
       <c r="B122" s="1">
-        <v>141.3</v>
+        <v>141.30000000000001</v>
       </c>
       <c r="C122" s="1">
         <v>26.8</v>
@@ -2151,9 +2474,9 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
-        <v>122.0</v>
+        <v>122</v>
       </c>
       <c r="B123" s="1">
         <v>18.8</v>
@@ -2165,15 +2488,15 @@
         <v>50.4</v>
       </c>
       <c r="E123" s="1">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="124">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>123.0</v>
+        <v>123</v>
       </c>
       <c r="B124" s="1">
-        <v>224.0</v>
+        <v>224</v>
       </c>
       <c r="C124" s="1">
         <v>2.4</v>
@@ -2185,9 +2508,9 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>124.0</v>
+        <v>124</v>
       </c>
       <c r="B125" s="1">
         <v>123.1</v>
@@ -2202,15 +2525,15 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="B126" s="1">
         <v>229.5</v>
       </c>
       <c r="C126" s="1">
-        <v>32.3</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="D126" s="1">
         <v>74.2</v>
@@ -2219,9 +2542,9 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
-        <v>126.0</v>
+        <v>126</v>
       </c>
       <c r="B127" s="1">
         <v>87.2</v>
@@ -2236,9 +2559,9 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>127.0</v>
+        <v>127</v>
       </c>
       <c r="B128" s="1">
         <v>7.8</v>
@@ -2253,32 +2576,32 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>128.0</v>
+        <v>128</v>
       </c>
       <c r="B129" s="1">
         <v>80.2</v>
       </c>
       <c r="C129" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D129" s="1">
-        <v>9.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E129" s="1">
-        <v>8.8</v>
-      </c>
-    </row>
-    <row r="130">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
-        <v>129.0</v>
+        <v>129</v>
       </c>
       <c r="B130" s="1">
         <v>220.3</v>
       </c>
       <c r="C130" s="1">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="D130" s="1">
         <v>3.2</v>
@@ -2287,26 +2610,26 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="B131" s="1">
         <v>59.6</v>
       </c>
       <c r="C131" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="D131" s="1">
         <v>43.1</v>
       </c>
       <c r="E131" s="1">
-        <v>9.7</v>
-      </c>
-    </row>
-    <row r="132">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
-        <v>131.0</v>
+        <v>131</v>
       </c>
       <c r="B132" s="1">
         <v>0.7</v>
@@ -2315,15 +2638,15 @@
         <v>39.6</v>
       </c>
       <c r="D132" s="1">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E132" s="1">
         <v>1.6</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>132.0</v>
+        <v>132</v>
       </c>
       <c r="B133" s="1">
         <v>265.2</v>
@@ -2332,15 +2655,15 @@
         <v>2.9</v>
       </c>
       <c r="D133" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="E133" s="1">
         <v>12.7</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>133.0</v>
+        <v>133</v>
       </c>
       <c r="B134" s="1">
         <v>8.4</v>
@@ -2355,9 +2678,9 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
-        <v>134.0</v>
+        <v>134</v>
       </c>
       <c r="B135" s="1">
         <v>219.8</v>
@@ -2369,12 +2692,12 @@
         <v>45.1</v>
       </c>
       <c r="E135" s="1">
-        <v>19.6</v>
-      </c>
-    </row>
-    <row r="136">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>135.0</v>
+        <v>135</v>
       </c>
       <c r="B136" s="1">
         <v>36.9</v>
@@ -2383,21 +2706,21 @@
         <v>38.6</v>
       </c>
       <c r="D136" s="1">
-        <v>65.6</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="E136" s="1">
         <v>10.8</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>136.0</v>
+        <v>136</v>
       </c>
       <c r="B137" s="1">
         <v>48.3</v>
       </c>
       <c r="C137" s="1">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="D137" s="1">
         <v>8.5</v>
@@ -2406,26 +2729,26 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>137.0</v>
+        <v>137</v>
       </c>
       <c r="B138" s="1">
         <v>25.6</v>
       </c>
       <c r="C138" s="1">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="D138" s="1">
-        <v>9.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E138" s="1">
         <v>9.5</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>138.0</v>
+        <v>138</v>
       </c>
       <c r="B139" s="1">
         <v>273.7</v>
@@ -2440,12 +2763,12 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>139.0</v>
+        <v>139</v>
       </c>
       <c r="B140" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="C140" s="1">
         <v>25.9</v>
@@ -2457,9 +2780,9 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="B141" s="1">
         <v>184.9</v>
@@ -2474,15 +2797,15 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>141.0</v>
+        <v>141</v>
       </c>
       <c r="B142" s="1">
-        <v>73.4</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="C142" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="D142" s="1">
         <v>12.9</v>
@@ -2491,9 +2814,9 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>142.0</v>
+        <v>142</v>
       </c>
       <c r="B143" s="1">
         <v>193.7</v>
@@ -2502,32 +2825,32 @@
         <v>35.4</v>
       </c>
       <c r="D143" s="1">
-        <v>75.6</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="E143" s="1">
         <v>19.2</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>143.0</v>
+        <v>143</v>
       </c>
       <c r="B144" s="1">
         <v>220.5</v>
       </c>
       <c r="C144" s="1">
-        <v>33.2</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="D144" s="1">
         <v>37.9</v>
       </c>
       <c r="E144" s="1">
-        <v>20.1</v>
-      </c>
-    </row>
-    <row r="145">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>144.0</v>
+        <v>144</v>
       </c>
       <c r="B145" s="1">
         <v>104.6</v>
@@ -2542,9 +2865,9 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>145.0</v>
+        <v>145</v>
       </c>
       <c r="B146" s="1">
         <v>96.2</v>
@@ -2559,26 +2882,26 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>146.0</v>
+        <v>146</v>
       </c>
       <c r="B147" s="1">
-        <v>140.3</v>
+        <v>140.30000000000001</v>
       </c>
       <c r="C147" s="1">
         <v>1.9</v>
       </c>
       <c r="D147" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="E147" s="1">
         <v>10.3</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>147.0</v>
+        <v>147</v>
       </c>
       <c r="B148" s="1">
         <v>240.1</v>
@@ -2587,21 +2910,21 @@
         <v>7.3</v>
       </c>
       <c r="D148" s="1">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E148" s="1">
         <v>13.2</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>148.0</v>
+        <v>148</v>
       </c>
       <c r="B149" s="1">
         <v>243.2</v>
       </c>
       <c r="C149" s="1">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="D149" s="1">
         <v>44.3</v>
@@ -2610,15 +2933,15 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>149.0</v>
+        <v>149</v>
       </c>
       <c r="B150" s="1">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C150" s="1">
-        <v>40.3</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="D150" s="1">
         <v>11.9</v>
@@ -2627,9 +2950,9 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="B151" s="1">
         <v>44.7</v>
@@ -2644,9 +2967,9 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>151.0</v>
+        <v>151</v>
       </c>
       <c r="B152" s="1">
         <v>280.7</v>
@@ -2655,18 +2978,18 @@
         <v>13.9</v>
       </c>
       <c r="D152" s="1">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="E152" s="1">
-        <v>16.1</v>
-      </c>
-    </row>
-    <row r="153">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
-        <v>152.0</v>
+        <v>152</v>
       </c>
       <c r="B153" s="1">
-        <v>121.0</v>
+        <v>121</v>
       </c>
       <c r="C153" s="1">
         <v>8.4</v>
@@ -2678,9 +3001,9 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
-        <v>153.0</v>
+        <v>153</v>
       </c>
       <c r="B154" s="1">
         <v>197.6</v>
@@ -2692,29 +3015,29 @@
         <v>14.2</v>
       </c>
       <c r="E154" s="1">
-        <v>16.6</v>
-      </c>
-    </row>
-    <row r="155">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
-        <v>154.0</v>
+        <v>154</v>
       </c>
       <c r="B155" s="1">
         <v>171.3</v>
       </c>
       <c r="C155" s="1">
-        <v>39.7</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="D155" s="1">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="E155" s="1">
-        <v>19.0</v>
-      </c>
-    </row>
-    <row r="156">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
-        <v>155.0</v>
+        <v>155</v>
       </c>
       <c r="B156" s="1">
         <v>187.8</v>
@@ -2729,12 +3052,12 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
-        <v>156.0</v>
+        <v>156</v>
       </c>
       <c r="B157" s="1">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C157" s="1">
         <v>11.6</v>
@@ -2746,9 +3069,9 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>157.0</v>
+        <v>157</v>
       </c>
       <c r="B158" s="1">
         <v>93.9</v>
@@ -2763,12 +3086,12 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>158.0</v>
+        <v>158</v>
       </c>
       <c r="B159" s="1">
-        <v>149.8</v>
+        <v>149.80000000000001</v>
       </c>
       <c r="C159" s="1">
         <v>1.3</v>
@@ -2780,9 +3103,9 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>159.0</v>
+        <v>159</v>
       </c>
       <c r="B160" s="1">
         <v>11.7</v>
@@ -2797,15 +3120,15 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>160.0</v>
+        <v>160</v>
       </c>
       <c r="B161" s="1">
-        <v>131.7</v>
+        <v>131.69999999999999</v>
       </c>
       <c r="C161" s="1">
-        <v>18.4</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="D161" s="1">
         <v>34.6</v>
@@ -2814,15 +3137,15 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>161.0</v>
+        <v>161</v>
       </c>
       <c r="B162" s="1">
         <v>172.5</v>
       </c>
       <c r="C162" s="1">
-        <v>18.1</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="D162" s="1">
         <v>30.7</v>
@@ -2831,15 +3154,15 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="B163" s="1">
         <v>85.7</v>
       </c>
       <c r="C163" s="1">
-        <v>35.8</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="D163" s="1">
         <v>49.3</v>
@@ -2848,15 +3171,15 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>163.0</v>
+        <v>163</v>
       </c>
       <c r="B164" s="1">
         <v>188.4</v>
       </c>
       <c r="C164" s="1">
-        <v>18.1</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="D164" s="1">
         <v>25.6</v>
@@ -2865,26 +3188,26 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>164.0</v>
+        <v>164</v>
       </c>
       <c r="B165" s="1">
         <v>163.5</v>
       </c>
       <c r="C165" s="1">
-        <v>36.8</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="D165" s="1">
         <v>7.4</v>
       </c>
       <c r="E165" s="1">
-        <v>18.0</v>
-      </c>
-    </row>
-    <row r="166">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>165.0</v>
+        <v>165</v>
       </c>
       <c r="B166" s="1">
         <v>117.2</v>
@@ -2899,9 +3222,9 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>166.0</v>
+        <v>166</v>
       </c>
       <c r="B167" s="1">
         <v>234.5</v>
@@ -2916,12 +3239,12 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>167.0</v>
+        <v>167</v>
       </c>
       <c r="B168" s="1">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C168" s="1">
         <v>37.6</v>
@@ -2930,12 +3253,12 @@
         <v>21.6</v>
       </c>
       <c r="E168" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="169">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>168.0</v>
+        <v>168</v>
       </c>
       <c r="B169" s="1">
         <v>206.8</v>
@@ -2944,15 +3267,15 @@
         <v>5.2</v>
       </c>
       <c r="D169" s="1">
-        <v>19.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="E169" s="1">
         <v>12.2</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>169.0</v>
+        <v>169</v>
       </c>
       <c r="B170" s="1">
         <v>215.4</v>
@@ -2964,12 +3287,12 @@
         <v>57.6</v>
       </c>
       <c r="E170" s="1">
-        <v>17.1</v>
-      </c>
-    </row>
-    <row r="171">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
-        <v>170.0</v>
+        <v>170</v>
       </c>
       <c r="B171" s="1">
         <v>284.3</v>
@@ -2981,29 +3304,29 @@
         <v>6.4</v>
       </c>
       <c r="E171" s="1">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="172">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>171.0</v>
+        <v>171</v>
       </c>
       <c r="B172" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="C172" s="1">
         <v>11.6</v>
       </c>
       <c r="D172" s="1">
-        <v>18.4</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="E172" s="1">
         <v>8.4</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>172.0</v>
+        <v>172</v>
       </c>
       <c r="B173" s="1">
         <v>164.5</v>
@@ -3018,26 +3341,26 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>173.0</v>
+        <v>173</v>
       </c>
       <c r="B174" s="1">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="C174" s="1">
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="D174" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="E174" s="1">
         <v>7.6</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
-        <v>174.0</v>
+        <v>174</v>
       </c>
       <c r="B175" s="1">
         <v>168.4</v>
@@ -3052,9 +3375,9 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
-        <v>175.0</v>
+        <v>175</v>
       </c>
       <c r="B176" s="1">
         <v>222.4</v>
@@ -3069,12 +3392,12 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>176.0</v>
+        <v>176</v>
       </c>
       <c r="B177" s="1">
-        <v>276.9</v>
+        <v>276.89999999999998</v>
       </c>
       <c r="C177" s="1">
         <v>48.9</v>
@@ -3083,12 +3406,12 @@
         <v>41.8</v>
       </c>
       <c r="E177" s="1">
-        <v>27.0</v>
-      </c>
-    </row>
-    <row r="178">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
-        <v>177.0</v>
+        <v>177</v>
       </c>
       <c r="B178" s="1">
         <v>248.4</v>
@@ -3103,9 +3426,9 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>178.0</v>
+        <v>178</v>
       </c>
       <c r="B179" s="1">
         <v>170.2</v>
@@ -3114,21 +3437,21 @@
         <v>7.8</v>
       </c>
       <c r="D179" s="1">
-        <v>35.2</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="E179" s="1">
         <v>11.7</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>179.0</v>
+        <v>179</v>
       </c>
       <c r="B180" s="1">
         <v>276.7</v>
       </c>
       <c r="C180" s="1">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D180" s="1">
         <v>23.7</v>
@@ -3137,26 +3460,26 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="B181" s="1">
         <v>165.6</v>
       </c>
       <c r="C181" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D181" s="1">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="E181" s="1">
         <v>12.6</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>181.0</v>
+        <v>181</v>
       </c>
       <c r="B182" s="1">
         <v>156.6</v>
@@ -3165,15 +3488,15 @@
         <v>2.6</v>
       </c>
       <c r="D182" s="1">
-        <v>8.3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E182" s="1">
         <v>10.5</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>182.0</v>
+        <v>182</v>
       </c>
       <c r="B183" s="1">
         <v>218.5</v>
@@ -3188,9 +3511,9 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>183.0</v>
+        <v>183</v>
       </c>
       <c r="B184" s="1">
         <v>56.2</v>
@@ -3202,18 +3525,18 @@
         <v>29.7</v>
       </c>
       <c r="E184" s="1">
-        <v>8.7</v>
-      </c>
-    </row>
-    <row r="185">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>184.0</v>
+        <v>184</v>
       </c>
       <c r="B185" s="1">
-        <v>287.6</v>
+        <v>287.60000000000002</v>
       </c>
       <c r="C185" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="D185" s="1">
         <v>71.8</v>
@@ -3222,9 +3545,9 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
-        <v>185.0</v>
+        <v>185</v>
       </c>
       <c r="B186" s="1">
         <v>253.8</v>
@@ -3233,32 +3556,32 @@
         <v>21.3</v>
       </c>
       <c r="D186" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="E186" s="1">
-        <v>17.6</v>
-      </c>
-    </row>
-    <row r="187">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>186.0</v>
+        <v>186</v>
       </c>
       <c r="B187" s="1">
-        <v>205.0</v>
+        <v>205</v>
       </c>
       <c r="C187" s="1">
         <v>45.1</v>
       </c>
       <c r="D187" s="1">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="E187" s="1">
         <v>22.6</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>187.0</v>
+        <v>187</v>
       </c>
       <c r="B188" s="1">
         <v>139.5</v>
@@ -3273,9 +3596,9 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
-        <v>188.0</v>
+        <v>188</v>
       </c>
       <c r="B189" s="1">
         <v>191.1</v>
@@ -3290,12 +3613,12 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
-        <v>189.0</v>
+        <v>189</v>
       </c>
       <c r="B190" s="1">
-        <v>286.0</v>
+        <v>286</v>
       </c>
       <c r="C190" s="1">
         <v>13.9</v>
@@ -3307,9 +3630,9 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>190.0</v>
+        <v>190</v>
       </c>
       <c r="B191" s="1">
         <v>18.7</v>
@@ -3324,9 +3647,9 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
-        <v>191.0</v>
+        <v>191</v>
       </c>
       <c r="B192" s="1">
         <v>39.5</v>
@@ -3341,9 +3664,9 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
-        <v>192.0</v>
+        <v>192</v>
       </c>
       <c r="B193" s="1">
         <v>75.5</v>
@@ -3352,21 +3675,21 @@
         <v>10.8</v>
       </c>
       <c r="D193" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="E193" s="1">
         <v>9.9</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
-        <v>193.0</v>
+        <v>193</v>
       </c>
       <c r="B194" s="1">
         <v>17.2</v>
       </c>
       <c r="C194" s="1">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D194" s="1">
         <v>31.6</v>
@@ -3375,46 +3698,46 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
-        <v>194.0</v>
+        <v>194</v>
       </c>
       <c r="B195" s="1">
         <v>166.8</v>
       </c>
       <c r="C195" s="1">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="D195" s="1">
         <v>3.6</v>
       </c>
       <c r="E195" s="1">
-        <v>19.6</v>
-      </c>
-    </row>
-    <row r="196">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
-        <v>195.0</v>
+        <v>195</v>
       </c>
       <c r="B196" s="1">
-        <v>149.7</v>
+        <v>149.69999999999999</v>
       </c>
       <c r="C196" s="1">
         <v>35.6</v>
       </c>
       <c r="D196" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="E196" s="1">
         <v>17.3</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
-        <v>196.0</v>
+        <v>196</v>
       </c>
       <c r="B197" s="1">
-        <v>38.2</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="C197" s="1">
         <v>3.7</v>
@@ -3426,32 +3749,32 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
-        <v>197.0</v>
+        <v>197</v>
       </c>
       <c r="B198" s="1">
         <v>94.2</v>
       </c>
       <c r="C198" s="1">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D198" s="1">
         <v>8.1</v>
       </c>
       <c r="E198" s="1">
-        <v>9.7</v>
-      </c>
-    </row>
-    <row r="199">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
-        <v>198.0</v>
+        <v>198</v>
       </c>
       <c r="B199" s="1">
-        <v>177.0</v>
+        <v>177</v>
       </c>
       <c r="C199" s="1">
-        <v>9.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D199" s="1">
         <v>6.4</v>
@@ -3460,15 +3783,15 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
-        <v>199.0</v>
+        <v>199</v>
       </c>
       <c r="B200" s="1">
-        <v>283.6</v>
+        <v>283.60000000000002</v>
       </c>
       <c r="C200" s="1">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="D200" s="1">
         <v>66.2</v>
@@ -3477,9 +3800,9 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="B201" s="1">
         <v>232.1</v>
@@ -3488,13 +3811,13 @@
         <v>8.6</v>
       </c>
       <c r="D201" s="1">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E201" s="1">
         <v>13.4</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>